<commit_message>
family drop location assignment via upload
</commit_message>
<xml_diff>
--- a/import_files/Family_Import_Test.xlsx
+++ b/import_files/Family_Import_Test.xlsx
@@ -11,13 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>family_id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
   <si>
     <t>first_name</t>
   </si>
@@ -46,6 +40,21 @@
     <t>family_code</t>
   </si>
   <si>
+    <t>drop_location</t>
+  </si>
+  <si>
+    <t>need1</t>
+  </si>
+  <si>
+    <t>need2</t>
+  </si>
+  <si>
+    <t>need3</t>
+  </si>
+  <si>
+    <t>need4</t>
+  </si>
+  <si>
     <t>Bill</t>
   </si>
   <si>
@@ -64,6 +73,21 @@
     <t>ASDF</t>
   </si>
   <si>
+    <t>oakland</t>
+  </si>
+  <si>
+    <t>bicycle</t>
+  </si>
+  <si>
+    <t>jeans</t>
+  </si>
+  <si>
+    <t>backpack</t>
+  </si>
+  <si>
+    <t>books</t>
+  </si>
+  <si>
     <t>Sammy</t>
   </si>
   <si>
@@ -76,6 +100,9 @@
     <t>More Awesome</t>
   </si>
   <si>
+    <t>sneakers</t>
+  </si>
+  <si>
     <t>Franny</t>
   </si>
   <si>
@@ -86,15 +113,84 @@
   </si>
   <si>
     <t>Less Awesome</t>
+  </si>
+  <si>
+    <t>12 pack PBR</t>
+  </si>
+  <si>
+    <t>canned food</t>
+  </si>
+  <si>
+    <t>underwear</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Sweet</t>
+  </si>
+  <si>
+    <t>BCDE</t>
+  </si>
+  <si>
+    <t>richmond</t>
+  </si>
+  <si>
+    <t>bike</t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>socks</t>
+  </si>
+  <si>
+    <t>Kayla</t>
+  </si>
+  <si>
+    <t>Blah Blah Blah</t>
+  </si>
+  <si>
+    <t>teddy bear</t>
+  </si>
+  <si>
+    <t>dress</t>
+  </si>
+  <si>
+    <t>roller skates</t>
+  </si>
+  <si>
+    <t>Joe</t>
+  </si>
+  <si>
+    <t>Good Dad</t>
+  </si>
+  <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>job</t>
+  </si>
+  <si>
+    <t>friends</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
@@ -125,8 +221,11 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="1">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -144,125 +243,293 @@
   <sheetFormatPr customHeight="1" defaultColWidth="17.14" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1">
-      <c t="s" r="A1">
+      <c t="s" s="1" r="A1">
         <v>0</v>
       </c>
-      <c t="s" r="B1">
+      <c t="s" s="1" r="B1">
         <v>1</v>
       </c>
-      <c t="s" r="C1">
+      <c t="s" s="1" r="C1">
         <v>2</v>
       </c>
-      <c t="s" r="D1">
+      <c t="s" s="1" r="D1">
         <v>3</v>
       </c>
-      <c t="s" r="E1">
+      <c t="s" s="1" r="E1">
         <v>4</v>
       </c>
-      <c t="s" r="F1">
+      <c t="s" s="1" r="F1">
         <v>5</v>
       </c>
-      <c t="s" r="G1">
+      <c t="s" s="1" r="G1">
         <v>6</v>
       </c>
-      <c t="s" r="H1">
+      <c t="s" s="1" r="H1">
         <v>7</v>
       </c>
-      <c t="s" r="I1">
+      <c t="s" s="1" r="I1">
         <v>8</v>
       </c>
-      <c t="s" r="J1">
+      <c t="s" s="1" r="J1">
         <v>9</v>
       </c>
-      <c t="s" r="K1">
+      <c t="s" s="1" r="K1">
         <v>10</v>
       </c>
+      <c t="s" s="1" r="L1">
+        <v>11</v>
+      </c>
+      <c t="s" s="1" r="M1">
+        <v>12</v>
+      </c>
+      <c t="s" s="1" r="N1">
+        <v>13</v>
+      </c>
     </row>
     <row r="2">
+      <c t="s" r="A2">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
       <c t="s" r="C2">
-        <v>11</v>
-      </c>
-      <c r="D2">
-        <v>15</v>
+        <v>15</v>
+      </c>
+      <c t="s" r="D2">
+        <v>16</v>
       </c>
       <c t="s" r="E2">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c t="s" r="F2">
-        <v>13</v>
-      </c>
-      <c t="s" r="G2">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="G2">
+        <v>8</v>
       </c>
       <c t="s" r="H2">
-        <v>14</v>
-      </c>
-      <c r="I2">
-        <v>8</v>
+        <v>18</v>
+      </c>
+      <c t="s" r="I2">
+        <v>19</v>
       </c>
       <c t="s" r="J2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c t="s" r="K2">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c t="s" r="L2">
+        <v>22</v>
+      </c>
+      <c t="s" r="M2">
+        <v>23</v>
+      </c>
+      <c t="s" r="N2">
+        <v>24</v>
       </c>
     </row>
     <row r="3">
+      <c t="s" r="A3">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
       <c t="s" r="C3">
+        <v>15</v>
+      </c>
+      <c t="s" r="D3">
+        <v>26</v>
+      </c>
+      <c t="s" r="E3">
+        <v>27</v>
+      </c>
+      <c t="s" r="F3">
         <v>17</v>
       </c>
-      <c r="D3">
+      <c r="G3">
         <v>10</v>
       </c>
-      <c t="s" r="E3">
-        <v>12</v>
-      </c>
-      <c t="s" r="F3">
-        <v>18</v>
-      </c>
-      <c t="s" r="G3">
+      <c t="s" r="H3">
+        <v>28</v>
+      </c>
+      <c t="s" r="I3">
         <v>19</v>
-      </c>
-      <c t="s" r="H3">
-        <v>14</v>
-      </c>
-      <c r="I3">
-        <v>10</v>
       </c>
       <c t="s" r="J3">
         <v>20</v>
       </c>
       <c t="s" r="K3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>35</v>
+      </c>
+      <c t="s" r="C4">
+        <v>31</v>
+      </c>
+      <c t="s" r="D4">
+        <v>32</v>
+      </c>
+      <c t="s" r="E4">
         <v>16</v>
       </c>
-    </row>
-    <row r="4">
-      <c t="s" r="C4">
-        <v>21</v>
-      </c>
-      <c r="D4">
+      <c r="F4">
         <v>35</v>
       </c>
-      <c t="s" r="E4">
-        <v>22</v>
-      </c>
-      <c t="s" r="F4">
-        <v>23</v>
-      </c>
-      <c t="s" r="G4">
-        <v>13</v>
-      </c>
-      <c r="H4">
+      <c r="G4">
+        <v>15</v>
+      </c>
+      <c t="s" r="H4">
+        <v>33</v>
+      </c>
+      <c t="s" r="I4">
+        <v>19</v>
+      </c>
+      <c t="s" r="J4">
+        <v>20</v>
+      </c>
+      <c t="s" r="K4">
+        <v>34</v>
+      </c>
+      <c t="s" r="L4">
         <v>35</v>
       </c>
-      <c r="I4">
-        <v>15</v>
-      </c>
-      <c t="s" r="J4">
+      <c t="s" r="M4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5">
+      <c t="s" r="A5">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>15</v>
+      </c>
+      <c t="s" r="C5">
+        <v>15</v>
+      </c>
+      <c t="s" r="D5">
+        <v>27</v>
+      </c>
+      <c t="s" r="E5">
+        <v>16</v>
+      </c>
+      <c t="s" r="F5">
+        <v>17</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c t="s" r="H5">
+        <v>38</v>
+      </c>
+      <c t="s" r="I5">
+        <v>39</v>
+      </c>
+      <c t="s" r="J5">
+        <v>40</v>
+      </c>
+      <c t="s" r="K5">
+        <v>41</v>
+      </c>
+      <c t="s" r="L5">
+        <v>42</v>
+      </c>
+      <c t="s" r="M5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" r="A6">
+        <v>44</v>
+      </c>
+      <c r="B6">
+        <v>12</v>
+      </c>
+      <c t="s" r="C6">
+        <v>31</v>
+      </c>
+      <c t="s" r="D6">
+        <v>26</v>
+      </c>
+      <c t="s" r="E6">
+        <v>26</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+      <c t="s" r="H6">
+        <v>45</v>
+      </c>
+      <c t="s" r="I6">
+        <v>39</v>
+      </c>
+      <c t="s" r="J6">
+        <v>40</v>
+      </c>
+      <c t="s" r="K6">
+        <v>46</v>
+      </c>
+      <c t="s" r="L6">
+        <v>47</v>
+      </c>
+      <c t="s" r="M6">
+        <v>48</v>
+      </c>
+      <c t="s" r="N6">
         <v>24</v>
       </c>
-      <c t="s" r="K4">
+    </row>
+    <row r="7">
+      <c t="s" r="A7">
+        <v>49</v>
+      </c>
+      <c r="B7">
+        <v>41</v>
+      </c>
+      <c t="s" r="C7">
+        <v>15</v>
+      </c>
+      <c t="s" r="D7">
         <v>16</v>
+      </c>
+      <c t="s" r="E7">
+        <v>16</v>
+      </c>
+      <c t="s" r="F7">
+        <v>17</v>
+      </c>
+      <c r="G7">
+        <v>11</v>
+      </c>
+      <c t="s" r="H7">
+        <v>50</v>
+      </c>
+      <c t="s" r="I7">
+        <v>39</v>
+      </c>
+      <c t="s" r="J7">
+        <v>40</v>
+      </c>
+      <c t="s" r="K7">
+        <v>51</v>
+      </c>
+      <c t="s" r="L7">
+        <v>52</v>
+      </c>
+      <c t="s" r="M7">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>